<commit_message>
fecha y hora de actualización
</commit_message>
<xml_diff>
--- a/Resources/data/Versión_2.0/Retorno a la presencialidad_ Estados 2021 FINAL.xlsx
+++ b/Resources/data/Versión_2.0/Retorno a la presencialidad_ Estados 2021 FINAL.xlsx
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="533">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1808" uniqueCount="534">
   <si>
     <t>Etiquetas de fila</t>
   </si>
@@ -1368,6 +1368,9 @@
   </si>
   <si>
     <t>Cambio de estatus y nuevas fuentes</t>
+  </si>
+  <si>
+    <t>Baja California Norte</t>
   </si>
   <si>
     <t>30 de agosto</t>
@@ -6891,7 +6894,7 @@
   <dimension ref="A1:N48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -7029,22 +7032,22 @@
         <v>228</v>
       </c>
       <c r="C4" s="38" t="s">
-        <v>229</v>
+        <v>361</v>
       </c>
       <c r="D4" s="39" t="s">
         <v>353</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F4" t="s">
         <v>355</v>
       </c>
       <c r="G4" s="20" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="I4" t="s">
         <v>248</v>
@@ -7053,16 +7056,16 @@
         <v>248</v>
       </c>
       <c r="K4" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L4" s="71" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M4" s="8" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="N4" s="20" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="5" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
@@ -7082,10 +7085,10 @@
         <v>264</v>
       </c>
       <c r="F5" s="29" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G5" s="51" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="H5" s="50" t="s">
         <v>266</v>
@@ -7100,10 +7103,10 @@
         <v>0.788</v>
       </c>
       <c r="L5" s="73" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="M5" s="61" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="N5" s="83" t="s">
         <v>360</v>
@@ -7120,37 +7123,37 @@
         <v>233</v>
       </c>
       <c r="D6" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>264</v>
       </c>
       <c r="F6" t="s">
+        <v>369</v>
+      </c>
+      <c r="G6" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>375</v>
+      </c>
+      <c r="I6" t="s">
+        <v>248</v>
+      </c>
+      <c r="J6" t="s">
+        <v>248</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="L6" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="M6" s="84" t="s">
+        <v>377</v>
+      </c>
+      <c r="N6" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="G6" s="20" t="s">
-        <v>373</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>374</v>
-      </c>
-      <c r="I6" t="s">
-        <v>248</v>
-      </c>
-      <c r="J6" t="s">
-        <v>248</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="L6" s="20" t="s">
-        <v>375</v>
-      </c>
-      <c r="M6" s="84" t="s">
-        <v>376</v>
-      </c>
-      <c r="N6" s="20" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="7" ht="25" customHeight="1" spans="1:14">
@@ -7167,16 +7170,16 @@
         <v>353</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="F7" t="s">
         <v>355</v>
       </c>
       <c r="G7" s="52" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I7" t="s">
         <v>248</v>
@@ -7185,16 +7188,16 @@
         <v>248</v>
       </c>
       <c r="K7" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="M7" s="85" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="N7" s="20" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
     </row>
     <row r="8" ht="25" customHeight="1" spans="1:14">
@@ -7208,42 +7211,42 @@
         <v>237</v>
       </c>
       <c r="D8" s="39" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>264</v>
       </c>
       <c r="F8" t="s">
+        <v>369</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>384</v>
+      </c>
+      <c r="H8" s="53" t="s">
+        <v>385</v>
+      </c>
+      <c r="I8" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" t="s">
+        <v>248</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>365</v>
+      </c>
+      <c r="L8" s="74" t="s">
+        <v>386</v>
+      </c>
+      <c r="M8" s="85" t="s">
+        <v>387</v>
+      </c>
+      <c r="N8" s="20" t="s">
         <v>368</v>
-      </c>
-      <c r="G8" s="8" t="s">
-        <v>383</v>
-      </c>
-      <c r="H8" s="53" t="s">
-        <v>384</v>
-      </c>
-      <c r="I8" t="s">
-        <v>248</v>
-      </c>
-      <c r="J8" t="s">
-        <v>248</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>364</v>
-      </c>
-      <c r="L8" s="74" t="s">
-        <v>385</v>
-      </c>
-      <c r="M8" s="85" t="s">
-        <v>386</v>
-      </c>
-      <c r="N8" s="20" t="s">
-        <v>367</v>
       </c>
     </row>
     <row r="9" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A9" s="32" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B9" s="33" t="s">
         <v>238</v>
@@ -7255,16 +7258,16 @@
         <v>353</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F9" s="29" t="s">
         <v>355</v>
       </c>
       <c r="G9" s="54" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="H9" s="55" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I9" s="29" t="s">
         <v>248</v>
@@ -7276,10 +7279,10 @@
         <v>1</v>
       </c>
       <c r="L9" s="56" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M9" s="86" t="s">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N9" s="83" t="s">
         <v>360</v>
@@ -7287,7 +7290,7 @@
     </row>
     <row r="10" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A10" s="32" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B10" s="33" t="s">
         <v>240</v>
@@ -7299,16 +7302,16 @@
         <v>353</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F10" s="29" t="s">
         <v>355</v>
       </c>
       <c r="G10" s="56" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="H10" s="55" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I10" s="29" t="s">
         <v>251</v>
@@ -7320,10 +7323,10 @@
         <v>0.95</v>
       </c>
       <c r="L10" s="76" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M10" s="87" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="N10" s="83" t="s">
         <v>360</v>
@@ -7331,7 +7334,7 @@
     </row>
     <row r="11" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A11" s="32" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B11" s="33" t="s">
         <v>242</v>
@@ -7343,16 +7346,16 @@
         <v>353</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F11" s="29" t="s">
         <v>355</v>
       </c>
       <c r="G11" s="56" t="s">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="H11" s="50" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I11" s="29" t="s">
         <v>248</v>
@@ -7364,18 +7367,18 @@
         <v>100</v>
       </c>
       <c r="L11" s="54" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="M11" s="54" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="N11" s="51" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A12" s="41" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B12" s="42" t="s">
         <v>244</v>
@@ -7384,19 +7387,19 @@
         <v>245</v>
       </c>
       <c r="D12" s="43" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E12" s="16" t="s">
         <v>264</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G12" s="57" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="H12" s="58" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>264</v>
@@ -7408,18 +7411,18 @@
         <v>100</v>
       </c>
       <c r="L12" s="58" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M12" s="19" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N12" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" ht="25" customHeight="1" spans="1:14">
       <c r="A13" s="37" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B13" s="37" t="s">
         <v>246</v>
@@ -7437,7 +7440,7 @@
         <v>355</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="H13" s="8" t="s">
         <v>250</v>
@@ -7455,15 +7458,15 @@
         <v>252</v>
       </c>
       <c r="M13" s="20" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="N13" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="14" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A14" s="32" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B14" s="33" t="s">
         <v>254</v>
@@ -7472,7 +7475,7 @@
         <v>255</v>
       </c>
       <c r="D14" s="35" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E14" s="60" t="s">
         <v>257</v>
@@ -7481,7 +7484,7 @@
         <v>355</v>
       </c>
       <c r="G14" s="51" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="H14" s="61" t="s">
         <v>259</v>
@@ -7493,21 +7496,21 @@
         <v>248</v>
       </c>
       <c r="K14" s="50" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L14" s="61" t="s">
         <v>260</v>
       </c>
       <c r="M14" s="51" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="N14" s="83" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="15" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A15" s="32" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B15" s="33" t="s">
         <v>262</v>
@@ -7522,10 +7525,10 @@
         <v>266</v>
       </c>
       <c r="F15" s="29" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G15" s="51" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="H15" s="61" t="s">
         <v>268</v>
@@ -7543,15 +7546,15 @@
         <v>269</v>
       </c>
       <c r="M15" s="51" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="N15" s="83" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="16" ht="25" customHeight="1" spans="1:14">
       <c r="A16" s="37" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B16" s="37" t="s">
         <v>271</v>
@@ -7569,7 +7572,7 @@
         <v>355</v>
       </c>
       <c r="G16" s="20" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="H16" s="8" t="s">
         <v>275</v>
@@ -7581,27 +7584,27 @@
         <v>248</v>
       </c>
       <c r="K16" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L16" s="8" t="s">
         <v>276</v>
       </c>
       <c r="M16" s="20" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N16" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="17" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A17" s="32" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>278</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="D17" s="35" t="s">
         <v>353</v>
@@ -7613,7 +7616,7 @@
         <v>355</v>
       </c>
       <c r="G17" s="51" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="H17" s="61" t="s">
         <v>282</v>
@@ -7625,21 +7628,21 @@
         <v>248</v>
       </c>
       <c r="K17" s="50" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L17" s="61" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="M17" s="51" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="N17" s="83" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="18" ht="25" customHeight="1" spans="1:14">
       <c r="A18" s="37" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B18" s="37" t="s">
         <v>285</v>
@@ -7669,21 +7672,21 @@
         <v>248</v>
       </c>
       <c r="K18" s="16" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="L18" s="20" t="s">
         <v>290</v>
       </c>
       <c r="M18" s="20" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="N18" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="19" s="3" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A19" s="37" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>292</v>
@@ -7713,16 +7716,16 @@
         <v>248</v>
       </c>
       <c r="K19" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L19" s="65" t="s">
         <v>297</v>
       </c>
       <c r="M19" s="58" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="N19" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="20" ht="25" customHeight="1" spans="1:14">
@@ -7736,19 +7739,19 @@
         <v>300</v>
       </c>
       <c r="D20" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E20" s="20" t="s">
         <v>266</v>
       </c>
       <c r="F20" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G20" s="66" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="I20" t="s">
         <v>248</v>
@@ -7757,21 +7760,21 @@
         <v>248</v>
       </c>
       <c r="K20" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L20" s="20" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M20" s="20" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="N20" s="19" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
     </row>
     <row r="21" ht="25" customHeight="1" spans="1:14">
       <c r="A21" s="36" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B21" s="37" t="s">
         <v>304</v>
@@ -7780,19 +7783,19 @@
         <v>305</v>
       </c>
       <c r="D21" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F21" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G21" s="20" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="H21" s="58" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I21" t="s">
         <v>264</v>
@@ -7810,12 +7813,12 @@
         <v>308</v>
       </c>
       <c r="N21" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="22" ht="25" customHeight="1" spans="1:14">
       <c r="A22" s="36" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B22" s="37" t="s">
         <v>309</v>
@@ -7824,19 +7827,19 @@
         <v>310</v>
       </c>
       <c r="D22" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F22" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G22" s="20" t="s">
         <v>311</v>
       </c>
       <c r="H22" s="58" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I22" t="s">
         <v>248</v>
@@ -7848,18 +7851,18 @@
         <v>100</v>
       </c>
       <c r="L22" s="20" t="s">
+        <v>427</v>
+      </c>
+      <c r="M22" s="19" t="s">
+        <v>428</v>
+      </c>
+      <c r="N22" s="58" t="s">
         <v>426</v>
-      </c>
-      <c r="M22" s="19" t="s">
-        <v>427</v>
-      </c>
-      <c r="N22" s="58" t="s">
-        <v>425</v>
       </c>
     </row>
     <row r="23" ht="25" customHeight="1" spans="1:14">
       <c r="A23" s="36" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B23" s="37" t="s">
         <v>314</v>
@@ -7871,16 +7874,16 @@
         <v>353</v>
       </c>
       <c r="E23" s="63" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F23" t="s">
         <v>355</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="H23" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="I23" t="s">
         <v>251</v>
@@ -7892,18 +7895,18 @@
         <v>0.95</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="M23" s="20" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="N23" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="24" s="29" customFormat="1" ht="25" customHeight="1" spans="1:14">
       <c r="A24" s="32" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B24" s="33" t="s">
         <v>316</v>
@@ -7915,16 +7918,16 @@
         <v>353</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F24" s="29" t="s">
         <v>355</v>
       </c>
       <c r="G24" s="51" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="H24" s="61" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="I24" s="29" t="s">
         <v>248</v>
@@ -7936,18 +7939,18 @@
         <v>0.9527</v>
       </c>
       <c r="L24" s="61" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="M24" s="87" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="N24" s="83" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="25" ht="25" customHeight="1" spans="1:14">
       <c r="A25" s="36" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B25" s="37" t="s">
         <v>318</v>
@@ -7965,10 +7968,10 @@
         <v>355</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H25" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="I25" t="s">
         <v>248</v>
@@ -7980,18 +7983,18 @@
         <v>0.756</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="M25" s="85" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="N25" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="26" ht="25" customHeight="1" spans="1:14">
       <c r="A26" s="36" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B26" s="37" t="s">
         <v>320</v>
@@ -8000,22 +8003,22 @@
         <v>321</v>
       </c>
       <c r="D26" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E26" s="63" t="s">
         <v>266</v>
       </c>
       <c r="F26" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="H26" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I26" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J26" t="s">
         <v>248</v>
@@ -8024,18 +8027,18 @@
         <v>0.9</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="M26" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="N26" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="27" ht="25" customHeight="1" spans="1:14">
       <c r="A27" s="36" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B27" s="37" t="s">
         <v>322</v>
@@ -8044,19 +8047,19 @@
         <v>323</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E27" s="63" t="s">
         <v>266</v>
       </c>
       <c r="F27" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="H27" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I27" t="s">
         <v>248</v>
@@ -8068,18 +8071,18 @@
         <v>0.9</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="N27" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="28" ht="25" customHeight="1" spans="1:14">
       <c r="A28" s="36" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="B28" s="37" t="s">
         <v>324</v>
@@ -8088,19 +8091,19 @@
         <v>325</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E28" s="63" t="s">
         <v>266</v>
       </c>
       <c r="F28" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="G28" s="20" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="H28" s="20" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="I28" t="s">
         <v>248</v>
@@ -8112,18 +8115,18 @@
         <v>0.87</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="M28" s="8" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="N28" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="29" ht="25" customHeight="1" spans="1:14">
       <c r="A29" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B29" s="37" t="s">
         <v>326</v>
@@ -8141,10 +8144,10 @@
         <v>355</v>
       </c>
       <c r="G29" s="8" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="H29" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I29" t="s">
         <v>248</v>
@@ -8153,21 +8156,21 @@
         <v>248</v>
       </c>
       <c r="K29" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M29" s="85" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="N29" s="58" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="30" ht="25" customHeight="1" spans="1:14">
       <c r="A30" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B30" s="37" t="s">
         <v>328</v>
@@ -8179,16 +8182,16 @@
         <v>353</v>
       </c>
       <c r="E30" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F30" t="s">
         <v>355</v>
       </c>
       <c r="G30" s="20" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="H30" s="20" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="I30" t="s">
         <v>248</v>
@@ -8197,21 +8200,21 @@
         <v>248</v>
       </c>
       <c r="K30" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L30" s="20" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="M30" s="20" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="N30" s="58" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="31" ht="25" customHeight="1" spans="1:14">
       <c r="A31" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B31" s="37" t="s">
         <v>330</v>
@@ -8223,16 +8226,16 @@
         <v>353</v>
       </c>
       <c r="E31" s="20" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="F31" t="s">
         <v>355</v>
       </c>
       <c r="G31" s="20" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="H31" s="20" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I31" t="s">
         <v>248</v>
@@ -8241,21 +8244,21 @@
         <v>248</v>
       </c>
       <c r="K31" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L31" s="20" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="M31" s="20" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="N31" s="58" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="32" ht="25" customHeight="1" spans="1:14">
       <c r="A32" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B32" s="37" t="s">
         <v>332</v>
@@ -8267,16 +8270,16 @@
         <v>353</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F32" t="s">
         <v>355</v>
       </c>
       <c r="G32" s="20" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="H32" s="20" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="I32" t="s">
         <v>248</v>
@@ -8285,21 +8288,21 @@
         <v>248</v>
       </c>
       <c r="K32" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L32" s="20" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="M32" s="20" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="N32" s="58" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="33" ht="25" customHeight="1" spans="1:14">
       <c r="A33" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B33" s="37" t="s">
         <v>334</v>
@@ -8311,16 +8314,16 @@
         <v>353</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F33" t="s">
         <v>355</v>
       </c>
       <c r="G33" s="20" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="H33" s="20" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="I33" t="s">
         <v>248</v>
@@ -8329,21 +8332,21 @@
         <v>248</v>
       </c>
       <c r="K33" s="16" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="L33" s="20" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M33" s="20" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N33" s="58" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="34" ht="25" customHeight="1" spans="1:14">
       <c r="A34" s="36" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B34" s="37" t="s">
         <v>336</v>
@@ -8352,19 +8355,19 @@
         <v>337</v>
       </c>
       <c r="D34" s="39" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="F34" t="s">
         <v>355</v>
       </c>
       <c r="G34" s="20" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="H34" s="8" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="I34" t="s">
         <v>248</v>
@@ -8376,13 +8379,13 @@
         <v>0.906</v>
       </c>
       <c r="L34" s="20" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="N34" s="58" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="36" spans="7:7">
@@ -8544,7 +8547,7 @@
       </c>
       <c r="E3" s="24"/>
       <c r="G3" s="20" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="H3" s="25" t="s">
         <v>289</v>
@@ -8562,7 +8565,7 @@
         <v>358</v>
       </c>
       <c r="M3" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" ht="99.75" spans="1:13">
@@ -8589,7 +8592,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="8"/>
       <c r="M4" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" ht="71.25" spans="1:13">
@@ -8603,7 +8606,7 @@
         <v>231</v>
       </c>
       <c r="D5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G5" s="8"/>
       <c r="I5" t="s">
@@ -8614,7 +8617,7 @@
       </c>
       <c r="K5" s="3"/>
       <c r="M5" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" ht="28.5" spans="1:13">
@@ -8628,7 +8631,7 @@
         <v>233</v>
       </c>
       <c r="D6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E6" s="8"/>
       <c r="G6" s="8"/>
@@ -8641,7 +8644,7 @@
       </c>
       <c r="K6" s="3"/>
       <c r="M6" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" ht="71.25" spans="1:13">
@@ -8666,7 +8669,7 @@
       <c r="K7" s="3"/>
       <c r="L7" s="8"/>
       <c r="M7" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" ht="128.25" spans="1:13">
@@ -8680,7 +8683,7 @@
         <v>237</v>
       </c>
       <c r="D8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -8693,12 +8696,12 @@
       <c r="K8" s="3"/>
       <c r="L8" s="21"/>
       <c r="M8" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" ht="28.5" spans="1:13">
       <c r="A9" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>238</v>
@@ -8707,7 +8710,7 @@
         <v>239</v>
       </c>
       <c r="D9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G9" s="8"/>
       <c r="I9" t="s">
@@ -8719,12 +8722,12 @@
       <c r="K9" s="3"/>
       <c r="L9" s="8"/>
       <c r="M9" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10" ht="28.5" spans="1:13">
       <c r="A10" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>240</v>
@@ -8733,7 +8736,7 @@
         <v>241</v>
       </c>
       <c r="D10" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G10" s="8"/>
       <c r="I10" t="s">
@@ -8745,12 +8748,12 @@
       <c r="K10" s="3"/>
       <c r="L10" s="8"/>
       <c r="M10" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" ht="28.5" spans="1:13">
       <c r="A11" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>242</v>
@@ -8759,7 +8762,7 @@
         <v>243</v>
       </c>
       <c r="D11" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G11" s="8"/>
       <c r="I11" t="s">
@@ -8771,12 +8774,12 @@
       <c r="K11" s="3"/>
       <c r="L11" s="8"/>
       <c r="M11" s="8" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>244</v>
@@ -8785,7 +8788,7 @@
         <v>245</v>
       </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="8"/>
@@ -8798,12 +8801,12 @@
       <c r="K12" s="3"/>
       <c r="L12" s="8"/>
       <c r="M12" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" ht="71.25" spans="1:13">
       <c r="A13" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>246</v>
@@ -8831,7 +8834,7 @@
     </row>
     <row r="14" ht="114" spans="1:13">
       <c r="A14" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>254</v>
@@ -8859,7 +8862,7 @@
     </row>
     <row r="15" ht="57" spans="1:13">
       <c r="A15" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>262</v>
@@ -8868,7 +8871,7 @@
         <v>263</v>
       </c>
       <c r="D15" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E15" s="8"/>
       <c r="G15" s="8"/>
@@ -8887,7 +8890,7 @@
     </row>
     <row r="16" ht="248.4" customHeight="1" spans="1:13">
       <c r="A16" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>271</v>
@@ -8915,7 +8918,7 @@
     </row>
     <row r="17" ht="128.25" spans="1:13">
       <c r="A17" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>278</v>
@@ -8924,7 +8927,7 @@
         <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E17" s="8"/>
       <c r="G17" s="8"/>
@@ -8943,7 +8946,7 @@
     </row>
     <row r="18" ht="85.5" spans="1:13">
       <c r="A18" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>285</v>
@@ -8971,7 +8974,7 @@
     </row>
     <row r="19" ht="28.5" spans="1:13">
       <c r="A19" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>292</v>
@@ -9008,7 +9011,7 @@
         <v>300</v>
       </c>
       <c r="D20" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E20" s="14"/>
       <c r="G20" s="8"/>
@@ -9027,7 +9030,7 @@
     </row>
     <row r="21" ht="99.75" spans="1:13">
       <c r="A21" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>304</v>
@@ -9036,7 +9039,7 @@
         <v>305</v>
       </c>
       <c r="D21" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E21" s="15"/>
       <c r="G21" s="8"/>
@@ -9055,7 +9058,7 @@
     </row>
     <row r="22" ht="28.5" spans="1:13">
       <c r="A22" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>309</v>
@@ -9064,7 +9067,7 @@
         <v>310</v>
       </c>
       <c r="D22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E22" s="15"/>
       <c r="G22" s="8"/>
@@ -9083,7 +9086,7 @@
     </row>
     <row r="23" spans="1:13">
       <c r="A23" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>314</v>
@@ -9106,12 +9109,12 @@
       <c r="K23" s="3"/>
       <c r="L23" s="8"/>
       <c r="M23" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>316</v>
@@ -9134,12 +9137,12 @@
       <c r="K24" s="3"/>
       <c r="L24" s="8"/>
       <c r="M24" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="25" ht="28.5" spans="1:13">
       <c r="A25" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>318</v>
@@ -9162,12 +9165,12 @@
       <c r="K25" s="3"/>
       <c r="L25" s="8"/>
       <c r="M25" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" ht="28.5" spans="1:13">
       <c r="A26" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>320</v>
@@ -9176,7 +9179,7 @@
         <v>321</v>
       </c>
       <c r="D26" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E26" s="8"/>
       <c r="G26" s="8"/>
@@ -9190,12 +9193,12 @@
       <c r="K26" s="3"/>
       <c r="L26" s="8"/>
       <c r="M26" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="27" ht="28.5" spans="1:13">
       <c r="A27" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>322</v>
@@ -9204,7 +9207,7 @@
         <v>323</v>
       </c>
       <c r="D27" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E27" s="8"/>
       <c r="G27" s="8"/>
@@ -9218,12 +9221,12 @@
       <c r="K27" s="3"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>324</v>
@@ -9232,7 +9235,7 @@
         <v>325</v>
       </c>
       <c r="D28" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="E28" s="8"/>
       <c r="G28" s="8"/>
@@ -9246,12 +9249,12 @@
       <c r="K28" s="3"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="29" ht="28.5" spans="1:13">
       <c r="A29" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>326</v>
@@ -9274,12 +9277,12 @@
       <c r="K29" s="3"/>
       <c r="L29" s="8"/>
       <c r="M29" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" spans="1:13">
       <c r="A30" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>328</v>
@@ -9302,12 +9305,12 @@
       <c r="K30" s="3"/>
       <c r="L30" s="8"/>
       <c r="M30" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="31" spans="1:13">
       <c r="A31" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>330</v>
@@ -9330,12 +9333,12 @@
       <c r="K31" s="3"/>
       <c r="L31" s="8"/>
       <c r="M31" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32" spans="1:13">
       <c r="A32" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>332</v>
@@ -9358,12 +9361,12 @@
       <c r="K32" s="3"/>
       <c r="L32" s="8"/>
       <c r="M32" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="33" spans="1:13">
       <c r="A33" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>334</v>
@@ -9386,12 +9389,12 @@
       <c r="K33" s="3"/>
       <c r="L33" s="8"/>
       <c r="M33" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="34" spans="1:13">
       <c r="A34" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>336</v>
@@ -9414,7 +9417,7 @@
       <c r="K34" s="3"/>
       <c r="L34" s="8"/>
       <c r="M34" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -9485,7 +9488,7 @@
         <v>345</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>347</v>
@@ -9517,13 +9520,13 @@
         <v>353</v>
       </c>
       <c r="D3" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E3" t="s">
         <v>256</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>357</v>
@@ -9538,10 +9541,10 @@
         <v>32</v>
       </c>
       <c r="K3" s="8" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
     </row>
     <row r="4" ht="128.25" spans="1:12">
@@ -9555,16 +9558,16 @@
         <v>353</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="E4" t="s">
         <v>32</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="H4" t="s">
         <v>32</v>
@@ -9576,10 +9579,10 @@
         <v>32</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="5" ht="71.25" spans="1:12">
@@ -9590,19 +9593,19 @@
         <v>231</v>
       </c>
       <c r="C5" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D5" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E5" t="s">
         <v>32</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="6" ht="57" spans="1:12">
@@ -9613,19 +9616,19 @@
         <v>233</v>
       </c>
       <c r="C6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="G6" s="17" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="H6" t="s">
         <v>32</v>
@@ -9637,7 +9640,7 @@
         <v>32</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="7" ht="71.25" spans="1:12">
@@ -9651,7 +9654,7 @@
         <v>353</v>
       </c>
       <c r="D7" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="E7" t="s">
         <v>256</v>
@@ -9666,10 +9669,10 @@
         <v>32</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="8" ht="171" spans="1:12">
@@ -9680,19 +9683,19 @@
         <v>237</v>
       </c>
       <c r="C8" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="D8" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="E8" t="s">
         <v>32</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="H8" t="s">
         <v>32</v>
@@ -9704,10 +9707,10 @@
         <v>32</v>
       </c>
       <c r="K8" s="21" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="9" ht="114" spans="1:12">
@@ -9718,19 +9721,19 @@
         <v>239</v>
       </c>
       <c r="C9" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D9" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="E9" t="s">
         <v>256</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G9" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H9" t="s">
         <v>256</v>
@@ -9742,10 +9745,10 @@
         <v>32</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10" ht="28.5" spans="1:12">
@@ -9756,19 +9759,19 @@
         <v>241</v>
       </c>
       <c r="C10" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D10" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E10" t="s">
         <v>32</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G10" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H10" t="s">
         <v>256</v>
@@ -9780,10 +9783,10 @@
         <v>256</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" ht="42.75" spans="1:12">
@@ -9794,34 +9797,34 @@
         <v>243</v>
       </c>
       <c r="C11" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D11" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="F11" s="18" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="G11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="I11" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="J11" t="s">
         <v>32</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="L11" s="18" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="12" ht="128.25" spans="1:12">
@@ -9832,16 +9835,16 @@
         <v>245</v>
       </c>
       <c r="C12" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D12" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="H12" t="s">
         <v>256</v>
@@ -9853,10 +9856,10 @@
         <v>32</v>
       </c>
       <c r="K12" s="8" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="13" ht="43.2" customHeight="1" spans="1:12">
@@ -9943,7 +9946,7 @@
         <v>263</v>
       </c>
       <c r="C15" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D15" s="8" t="s">
         <v>265</v>
@@ -10019,7 +10022,7 @@
         <v>125</v>
       </c>
       <c r="C17" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>279</v>
@@ -10133,7 +10136,7 @@
         <v>300</v>
       </c>
       <c r="C20" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>301</v>
@@ -10171,7 +10174,7 @@
         <v>305</v>
       </c>
       <c r="C21" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>301</v>
@@ -10209,7 +10212,7 @@
         <v>310</v>
       </c>
       <c r="C22" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D22" s="15" t="s">
         <v>301</v>
@@ -10250,14 +10253,14 @@
         <v>353</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E23" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F23" s="8"/>
       <c r="G23" s="8" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="H23" s="8" t="s">
         <v>36</v>
@@ -10269,10 +10272,10 @@
         <v>37</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="L23" s="8" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="24" ht="28.5" spans="1:12">
@@ -10286,16 +10289,16 @@
         <v>353</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>36</v>
       </c>
       <c r="F24" s="8" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="H24" s="8" t="s">
         <v>32</v>
@@ -10308,7 +10311,7 @@
       </c>
       <c r="K24" s="8"/>
       <c r="L24" s="8" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="25" ht="156.75" spans="1:12">
@@ -10322,16 +10325,16 @@
         <v>353</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H25" s="8" t="s">
         <v>32</v>
@@ -10343,10 +10346,10 @@
         <v>37</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="L25" s="8" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="26" ht="99.75" spans="1:12">
@@ -10357,22 +10360,22 @@
         <v>321</v>
       </c>
       <c r="C26" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H26" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="I26" s="8" t="s">
         <v>32</v>
@@ -10381,10 +10384,10 @@
         <v>37</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="L26" s="8" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="27" ht="114" spans="1:12">
@@ -10395,19 +10398,19 @@
         <v>323</v>
       </c>
       <c r="C27" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="G27" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H27" s="8" t="s">
         <v>32</v>
@@ -10419,10 +10422,10 @@
         <v>37</v>
       </c>
       <c r="K27" s="8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="L27" s="8" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="28" ht="57" spans="1:12">
@@ -10433,17 +10436,17 @@
         <v>325</v>
       </c>
       <c r="C28" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F28" s="8"/>
       <c r="G28" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H28" s="8" t="s">
         <v>32</v>
@@ -10455,10 +10458,10 @@
         <v>37</v>
       </c>
       <c r="K28" s="8" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="L28" s="8" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="29" ht="85.5" spans="1:12">
@@ -10472,10 +10475,10 @@
         <v>353</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F29" s="8"/>
       <c r="G29" s="8"/>
@@ -10489,10 +10492,10 @@
         <v>37</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="L29" s="8" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="30" ht="57" spans="1:12">
@@ -10509,11 +10512,11 @@
         <v>32</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F30" s="8"/>
       <c r="G30" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H30" s="8" t="s">
         <v>32</v>
@@ -10525,10 +10528,10 @@
         <v>37</v>
       </c>
       <c r="K30" s="20" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="L30" s="8" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="31" ht="71.25" spans="1:12">
@@ -10542,14 +10545,14 @@
         <v>353</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F31" s="8"/>
       <c r="G31" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="H31" s="8" t="s">
         <v>32</v>
@@ -10561,10 +10564,10 @@
         <v>37</v>
       </c>
       <c r="K31" s="20" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="L31" s="8" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
     </row>
     <row r="32" ht="185.25" spans="1:12">
@@ -10578,14 +10581,14 @@
         <v>353</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>32</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="H32" s="8" t="s">
         <v>32</v>
@@ -10597,10 +10600,10 @@
         <v>37</v>
       </c>
       <c r="K32" s="20" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="L32" s="8" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="33" ht="85.5" spans="1:12">
@@ -10614,14 +10617,14 @@
         <v>353</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E33" s="8" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="8" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="H33" s="8" t="s">
         <v>32</v>
@@ -10633,10 +10636,10 @@
         <v>37</v>
       </c>
       <c r="K33" s="20" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="L33" s="8" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="34" ht="99.75" spans="1:12">
@@ -10650,7 +10653,7 @@
         <v>353</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>32</v>
@@ -10667,10 +10670,10 @@
         <v>37</v>
       </c>
       <c r="K34" s="8" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="L34" s="8" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -10715,7 +10718,7 @@
         <v>345</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>347</v>
@@ -10752,7 +10755,7 @@
         <v>251</v>
       </c>
       <c r="E5" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="H5" s="2" t="s">
         <v>251</v>
@@ -10760,7 +10763,7 @@
     </row>
     <row r="6" spans="3:8">
       <c r="C6" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>264</v>
@@ -10768,10 +10771,10 @@
     </row>
     <row r="7" spans="3:8">
       <c r="C7" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
     </row>
   </sheetData>

</xml_diff>